<commit_message>
Update with alternate resistor values
for microBOM
</commit_message>
<xml_diff>
--- a/BOM/microBOM-RevA.xlsx
+++ b/BOM/microBOM-RevA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="96">
   <si>
     <t>TESA - Industrial Design Project - Summer 2014</t>
   </si>
@@ -90,9 +90,6 @@
     <t>R104,R105</t>
   </si>
   <si>
-    <t>1.42k</t>
-  </si>
-  <si>
     <t>C101,C104</t>
   </si>
   <si>
@@ -253,6 +250,62 @@
   </si>
   <si>
     <t>0.282/0.247/0.223</t>
+  </si>
+  <si>
+    <t>667-ERJ-U03F1001V</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>1.2k</t>
+  </si>
+  <si>
+    <t>1.4k</t>
+  </si>
+  <si>
+    <t>1.6k</t>
+  </si>
+  <si>
+    <t>1.8k</t>
+  </si>
+  <si>
+    <t>ERJ-U03F1001V</t>
+  </si>
+  <si>
+    <t>0.129/0.059/--</t>
+  </si>
+  <si>
+    <t>667-ERJ-3GEYJ122V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3GEYJ122V
+</t>
+  </si>
+  <si>
+    <t>0.023/0.012/0.007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+667-ERJ-S03F1401V </t>
+  </si>
+  <si>
+    <t>ERJ-S03F1401V</t>
+  </si>
+  <si>
+    <t>0.164/0.069/0.05</t>
+  </si>
+  <si>
+    <t>667-ERJ-3GEYJ162V</t>
+  </si>
+  <si>
+    <t>ERJ-3GEYJ162V</t>
+  </si>
+  <si>
+    <t>667-ERJ-3GEYJ182V</t>
+  </si>
+  <si>
+    <t>ERJ-3GEYJ182V</t>
   </si>
 </sst>
 </file>
@@ -294,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -302,6 +355,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J36"/>
+  <dimension ref="A3:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +732,7 @@
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -686,10 +746,10 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I9" t="s">
         <v>14</v>
@@ -706,25 +766,25 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
         <v>34</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" t="s">
         <v>35</v>
       </c>
-      <c r="H10" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" t="s">
-        <v>36</v>
-      </c>
       <c r="J10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -732,270 +792,401 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="H12" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" t="s">
-        <v>51</v>
+        <v>33</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="H13" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="H14" t="s">
-        <v>45</v>
-      </c>
-      <c r="I14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J14" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="H15" t="s">
-        <v>45</v>
-      </c>
-      <c r="I15" t="s">
-        <v>49</v>
-      </c>
-      <c r="J15" t="s">
-        <v>50</v>
+        <v>36</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G16" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="H16" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="I16" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="J16" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G17" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I17" t="s">
-        <v>77</v>
+        <v>51</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="J17" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
       </c>
       <c r="F18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G18" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="H18" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="I18" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="J18" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" t="s">
+        <v>44</v>
+      </c>
+      <c r="I20" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" t="s">
+        <v>76</v>
+      </c>
+      <c r="J21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" t="s">
+        <v>60</v>
+      </c>
+      <c r="J22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>4</v>
       </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" t="s">
         <v>63</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H23" t="s">
         <v>64</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I23" t="s">
         <v>65</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J23" t="s">
         <v>66</v>
       </c>
-      <c r="J19" t="s">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C24" t="s">
         <v>69</v>
       </c>
-      <c r="B20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="F24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" t="s">
         <v>70</v>
       </c>
-      <c r="F20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="H24" t="s">
         <v>71</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I24" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="J24" t="s">
         <v>73</v>
       </c>
-      <c r="J20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I30" s="1"/>
-    </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I36" s="2"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="1"/>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
BOM corrections and update rev
The power BOM was completely wrong, so I re-made it; the others just had
their boards and revs updated
</commit_message>
<xml_diff>
--- a/BOM/microBOM-RevA.xlsx
+++ b/BOM/microBOM-RevA.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\GitHub\Tesa\BOM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="180" windowWidth="8595" windowHeight="6915"/>
   </bookViews>
@@ -426,7 +421,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -461,7 +456,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -672,14 +667,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>

</xml_diff>

<commit_message>
Made an inventory and acquisitions list
New directory for inventory and acquisitions! This must be updated every
time a component is used!!!!!!! Moved the previous orders to a new
directory in the hope they will never be copied. readme updated.
</commit_message>
<xml_diff>
--- a/BOM/microBOM-RevA.xlsx
+++ b/BOM/microBOM-RevA.xlsx
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>